<commit_message>
created more parsers and instrument for find by tag
</commit_message>
<xml_diff>
--- a/practice-parsing/output/rfglobalnet.xlsx
+++ b/practice-parsing/output/rfglobalnet.xlsx
@@ -451,57 +451,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>How RAD-Hard Technologies Make Space Exploration A Reality</t>
+          <t>Cryogenic Microwave Wafer-Scale Characterization Of Superconducting Resonators</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7/3/2024</t>
+          <t>7/9/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Discover how RAD-Hard technologies revolutionize space exploration. Overcoming radiation challenges, they power satellites and missions to shape the future of planetary exploration and global communications.</t>
+          <t>In quantum computing, superconducting resonators are pivotal in enabling qubit readout and interaction. Explore their characterization at cryogenic temperatures using advanced wafer-scale measurement techniques.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RAD-Hard (ORG)</t>
+          <t>quantum (ORG)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/from-sci-fi-to-sci-fact-how-rad-hard-technologies-make-space-exploration-a-reality-0001</t>
+          <t>https://www.rfglobalnet.com/doc/cryogenic-microwave-wafer-scale-characterization-of-superconducting-resonators-0001</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>How To Select Power Amplifiers For High-Frequency mmWave Applications</t>
+          <t>How RAD-Hard Technologies Make Space Exploration A Reality</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7/1/2024</t>
+          <t>7/3/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Explore some of the challenges in finding reliable power amplifiers that operate at high frequencies and how SWaP-C and lead time challenges can be addressed.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>Discover how RAD-Hard technologies revolutionize space exploration. Overcoming radiation challenges, they power satellites and missions to shape the future of planetary exploration and global communications.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>RAD-Hard (ORG)</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/how-to-select-power-amplifiers-for-high-frequency-millimeter-wave-applications-0001</t>
+          <t>https://www.rfglobalnet.com/doc/from-sci-fi-to-sci-fact-how-rad-hard-technologies-make-space-exploration-a-reality-0001</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Monitor Radio Spectrum While Hunting Interference</t>
+          <t>How To Select Power Amplifiers For High-Frequency mmWave Applications</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -511,128 +515,124 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>As the RF spectrum becomes increasingly congested, interference issues rise. Explore the crucial role of spectrum analyzers in identifying and mitigating interference for reliable wireless communication.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>RF (ORG)</t>
-        </is>
-      </c>
+          <t>Explore some of the challenges in finding reliable power amplifiers that operate at high frequencies and how SWaP-C and lead time challenges can be addressed.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/monitor-radio-spectrum-while-hunting-interference-0001</t>
+          <t>https://www.rfglobalnet.com/doc/how-to-select-power-amplifiers-for-high-frequency-millimeter-wave-applications-0001</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Flexibility Of Multilayer Ceramic Capacitors</t>
+          <t>Monitor Radio Spectrum While Hunting Interference</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6/28/2024</t>
+          <t>7/1/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Increasing demands for automotive electronics drive the need for resilient components. Discover how FlexiCap™ ensures flexibility in AEC-Q200-certified MLCCs for enhanced reliability under harsh conditions.</t>
+          <t>As the RF spectrum becomes increasingly congested, interference issues rise. Explore the crucial role of spectrum analyzers in identifying and mitigating interference for reliable wireless communication.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>FlexiCap (WORK_OF_ART), AEC-Q200 (ORG)</t>
+          <t>RF (ORG)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/flexibility-of-multilayer-ceramic-capacitors-guaranteed-mm-of-bend-on-aec-q-certified-components-0001</t>
+          <t>https://www.rfglobalnet.com/doc/monitor-radio-spectrum-while-hunting-interference-0001</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Trends In Battery Energy Storage Systems</t>
+          <t>Flexibility Of Multilayer Ceramic Capacitors</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6/26/2024</t>
+          <t>6/28/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Battery Energy Storage Systems (BESS) are pivotal in modern energy infrastructure. Explore their components, advantages, and challenges amid evolving global energy dynamics.</t>
+          <t>Increasing demands for automotive electronics drive the need for resilient components. Discover how FlexiCap™ ensures flexibility in AEC-Q200-certified MLCCs for enhanced reliability under harsh conditions.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Battery Energy Storage Systems (ORG)</t>
+          <t>FlexiCap (WORK_OF_ART), AEC-Q200 (ORG)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/trends-in-battery-energy-storage-systems-0001</t>
+          <t>https://www.rfglobalnet.com/doc/flexibility-of-multilayer-ceramic-capacitors-guaranteed-mm-of-bend-on-aec-q-certified-components-0001</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Power Conversion Capacitors For Harsh Environments</t>
+          <t>Trends In Battery Energy Storage Systems</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>6/26/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Explore the pivotal role of capacitors in power conversion circuits, their specific requirements, and the characteristics necessary for their reliable operation in demanding environments. </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>Battery Energy Storage Systems (BESS) are pivotal in modern energy infrastructure. Explore their components, advantages, and challenges amid evolving global energy dynamics.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Battery Energy Storage Systems (ORG)</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/power-conversion-capacitors-for-harsh-environments-0001</t>
+          <t>https://www.rfglobalnet.com/doc/trends-in-battery-energy-storage-systems-0001</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>The Future Of Positioning: Exploring UWB And Bluetooth Channel Sounding</t>
+          <t>Power Conversion Capacitors For Harsh Environments</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/20/2024</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Discover the advancements in Ultra-Wideband (UWB) and Bluetooth channel sounding that provide distinct advantages and solutions for precise location tracking.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Ultra-Wideband (GPE)</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Explore the pivotal role of capacitors in power conversion circuits, their specific requirements, and the characteristics necessary for their reliable operation in demanding environments. </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-future-of-positioning-exploring-uwb-and-bluetooth-channel-sounding-0001</t>
+          <t>https://www.rfglobalnet.com/doc/power-conversion-capacitors-for-harsh-environments-0001</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>How Modern LEO Satellite Technologies Are Changing The Space Race</t>
+          <t>The Future Of Positioning: Exploring UWB And Bluetooth Channel Sounding</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -642,78 +642,78 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Low Earth Orbit (LEO) technologies are reshaping the space race with enhanced global connectivity and data accessibility, marking a pivotal shift in satellite deployment strategies.</t>
+          <t>Discover the advancements in Ultra-Wideband (UWB) and Bluetooth channel sounding that provide distinct advantages and solutions for precise location tracking.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LEO (ORG)</t>
+          <t>Ultra-Wideband (GPE)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/how-modern-leo-satellite-technologies-are-changing-the-space-race-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-future-of-positioning-exploring-uwb-and-bluetooth-channel-sounding-0001</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>How Do You Use A VNA?</t>
+          <t>How Modern LEO Satellite Technologies Are Changing The Space Race</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/19/2024</t>
+          <t>6/20/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Delve into how vector network analyzers (VNAs) are employed across various applications to ensure accurate measurements crucial for optimizing and troubleshooting complex RF systems.</t>
+          <t>Low Earth Orbit (LEO) technologies are reshaping the space race with enhanced global connectivity and data accessibility, marking a pivotal shift in satellite deployment strategies.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>RF (ORG)</t>
+          <t>LEO (ORG)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/how-do-you-use-a-vna-0001</t>
+          <t>https://www.rfglobalnet.com/doc/how-modern-leo-satellite-technologies-are-changing-the-space-race-0001</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Visit Booth #704 At IMS 2024 For Solutions Spanning Active Load Pull To RF Channel Emulation</t>
+          <t>How Do You Use A VNA?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6/14/2024</t>
+          <t>6/19/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>In booth 704, Maury Microwave will showcase its latest products and solutions, many of which are used in several in-booth demonstrations ranging from active load pull for 6G and sub-THz frequencies to cryogenic noise parameters to 5G non-terrestrial network (NTN) link emulation. In this blog post, discover why booth 704 is a key destination for IMS attendees.</t>
+          <t>Delve into how vector network analyzers (VNAs) are employed across various applications to ensure accurate measurements crucial for optimizing and troubleshooting complex RF systems.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>704 (CARDINAL), Maury Microwave (PERSON), 6 (CARDINAL), 5 (CARDINAL), NTN (ORG), 704 (CARDINAL), IMS (ORG)</t>
+          <t>RF (ORG)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/visit-booth-at-ims-for-solutions-spanning-active-load-pull-to-rf-channel-emulation-0001</t>
+          <t>https://www.rfglobalnet.com/doc/how-do-you-use-a-vna-0001</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>The Enduring Importance Of Analog Signal Processing In Defense</t>
+          <t>Visit Booth #704 At IMS 2024 For Solutions Spanning Active Load Pull To RF Channel Emulation</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -723,20 +723,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Explore why, amidst digital dominance, analog remains crucial for resilience, high-frequency applications, and interfacing with the physical world in military technology.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>In booth 704, Maury Microwave will showcase its latest products and solutions, many of which are used in several in-booth demonstrations ranging from active load pull for 6G and sub-THz frequencies to cryogenic noise parameters to 5G non-terrestrial network (NTN) link emulation. In this blog post, discover why booth 704 is a key destination for IMS attendees.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>704 (CARDINAL), Maury Microwave (PERSON), 6 (CARDINAL), 5 (CARDINAL), NTN (ORG), 704 (CARDINAL), IMS (ORG)</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-enduring-importance-of-analog-signal-processing-in-defense-0001</t>
+          <t>https://www.rfglobalnet.com/doc/visit-booth-at-ims-for-solutions-spanning-active-load-pull-to-rf-channel-emulation-0001</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Startup Spotlight: Thintronics Debuts At IMS</t>
+          <t>The Enduring Importance Of Analog Signal Processing In Defense</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -746,24 +750,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Discover how Thintronics Inc. is revolutionizing AI data centers and RF technologies with its advanced insulation platform at IMS2024. Visit Booth #2343 to explore cutting-edge solutions for high-performance applications.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>AI (ORG), RF (ORG)</t>
-        </is>
-      </c>
+          <t>Explore why, amidst digital dominance, analog remains crucial for resilience, high-frequency applications, and interfacing with the physical world in military technology.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/startup-spotlight-thintronics-debuts-at-ims-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-enduring-importance-of-analog-signal-processing-in-defense-0001</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Selecting The Right Cable Assembly To Meet The Demands Of Commercial Space Applications</t>
+          <t>Startup Spotlight: Thintronics Debuts At IMS</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -773,51 +773,51 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Selecting the right cable assembly for commercial space applications, such as LEO satellites, demands robust, high-performance solutions able to withstand extreme conditions and ensure reliable operation.</t>
+          <t>Discover how Thintronics Inc. is revolutionizing AI data centers and RF technologies with its advanced insulation platform at IMS2024. Visit Booth #2343 to explore cutting-edge solutions for high-performance applications.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LEO (ORG)</t>
+          <t>AI (ORG), RF (ORG)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/selecting-the-right-cable-assembly-to-meet-the-demands-of-commercial-space-applications-0001</t>
+          <t>https://www.rfglobalnet.com/doc/startup-spotlight-thintronics-debuts-at-ims-0001</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Catch Up With Maury Microwave At IMS Booth 704</t>
+          <t>Selecting The Right Cable Assembly To Meet The Demands Of Commercial Space Applications</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6/12/2024</t>
+          <t>6/14/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Maury Microwave invites you to booth #704 at IMS 2024 for an array of in-booth demonstrations and seminars. Explore our latest products and capabilities, including active device characterization up to 330 GHz and cryogenic noise parameter measurements.</t>
+          <t>Selecting the right cable assembly for commercial space applications, such as LEO satellites, demands robust, high-performance solutions able to withstand extreme conditions and ensure reliable operation.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Maury Microwave (PERSON), 704 (MONEY), IMS 2024 (DATE), up to (CARDINAL), 330 GHz (CARDINAL)</t>
+          <t>LEO (ORG)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/catch-up-with-maury-microwave-at-booth-704-0001</t>
+          <t>https://www.rfglobalnet.com/doc/selecting-the-right-cable-assembly-to-meet-the-demands-of-commercial-space-applications-0001</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Unlocking Endurance With MEMS Technology: Extending Relay Lifespan By 1000x</t>
+          <t>Catch Up With Maury Microwave At IMS Booth 704</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -827,24 +827,24 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Explore how innovative Ideal Switch technology is setting new benchmarks for reliability and efficiency in semiconductor testing.</t>
+          <t>Maury Microwave invites you to booth #704 at IMS 2024 for an array of in-booth demonstrations and seminars. Explore our latest products and capabilities, including active device characterization up to 330 GHz and cryogenic noise parameter measurements.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ideal Switch (ORG)</t>
+          <t>Maury Microwave (PERSON), 704 (MONEY), IMS 2024 (DATE), up to (CARDINAL), 330 GHz (CARDINAL)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/unlocking-endurance-with-mems-technology-extending-relay-lifespan-by-x-0001</t>
+          <t>https://www.rfglobalnet.com/doc/catch-up-with-maury-microwave-at-booth-704-0001</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Alleviating Bottlenecks With Low-Loss Dielectric Fixturing</t>
+          <t>Unlocking Endurance With MEMS Technology: Extending Relay Lifespan By 1000x</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -854,74 +854,74 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Explore how Menlo Micro utilized printable dielectric fixtures to address challenges in the development and testing of their RF and DC switches.</t>
+          <t>Explore how innovative Ideal Switch technology is setting new benchmarks for reliability and efficiency in semiconductor testing.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Menlo Micro (ORG), DC (GPE)</t>
+          <t>Ideal Switch (ORG)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/menlo-micro-alleviates-product-design-and-test-feedback-cycle-bottlenecks-with-low-loss-dielectric-fixturing-0001</t>
+          <t>https://www.rfglobalnet.com/doc/unlocking-endurance-with-mems-technology-extending-relay-lifespan-by-x-0001</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Group Delay Engineering In RF Filters</t>
+          <t>Alleviating Bottlenecks With Low-Loss Dielectric Fixturing</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6/6/2024</t>
+          <t>6/12/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>RF filter design can be tricky, especially in mid-range frequencies where impedance matching and parasitics pose challenges. Explore the complexities and methods to engineer optimal group delay curves.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+          <t>Explore how Menlo Micro utilized printable dielectric fixtures to address challenges in the development and testing of their RF and DC switches.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Menlo Micro (ORG), DC (GPE)</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/group-delay-engineering-in-rf-filters-0001</t>
+          <t>https://www.rfglobalnet.com/doc/menlo-micro-alleviates-product-design-and-test-feedback-cycle-bottlenecks-with-low-loss-dielectric-fixturing-0001</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mastering 5G Reliability: Safeguarding Your Network Infrastructure</t>
+          <t>Group Delay Engineering In RF Filters</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6/5/2024</t>
+          <t>6/6/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5G promises unprecedented speed, lower latency, and more capabilities to support new and emerging technologies. However, protecting the 5G network infrastructure brings additional cybersecurity challenges, requiring operators and other communications industry professionals to plan additional safeguards. Having the dangers of the 5G infrastructure explained in clear language allows proactivity and avoids vulnerabilities.</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>5 (CARDINAL), 5 (CARDINAL), 5 (CARDINAL)</t>
-        </is>
-      </c>
+          <t>RF filter design can be tricky, especially in mid-range frequencies where impedance matching and parasitics pose challenges. Explore the complexities and methods to engineer optimal group delay curves.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/mastering-g-reliability-safeguarding-your-network-infrastructure-0001</t>
+          <t>https://www.rfglobalnet.com/doc/group-delay-engineering-in-rf-filters-0001</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Quantum Computing: Top 5 Questions Answered</t>
+          <t>Mastering 5G Reliability: Safeguarding Your Network Infrastructure</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -931,24 +931,24 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Quantum computing, once confined to theory and sci-fi, is now at the forefront of innovation. Explore its real-world applications, challenges, and potential through these five essential questions.</t>
+          <t>5G promises unprecedented speed, lower latency, and more capabilities to support new and emerging technologies. However, protecting the 5G network infrastructure brings additional cybersecurity challenges, requiring operators and other communications industry professionals to plan additional safeguards. Having the dangers of the 5G infrastructure explained in clear language allows proactivity and avoids vulnerabilities.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Quantum (ORG), sci-fi (ORG), five (CARDINAL)</t>
+          <t>5 (CARDINAL), 5 (CARDINAL), 5 (CARDINAL)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/quantum-computing-top-questions-answered-0001</t>
+          <t>https://www.rfglobalnet.com/doc/mastering-g-reliability-safeguarding-your-network-infrastructure-0001</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>How To Manage Burgeoning Data Traffic On A Finite RF Spectrum</t>
+          <t>Quantum Computing: Top 5 Questions Answered</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -958,43 +958,47 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Explore strategies and innovations to unlock higher-frequency bandwidths, which are crucial for sustaining technological advancement and meeting the escalating demands of our connected future.</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
+          <t>Quantum computing, once confined to theory and sci-fi, is now at the forefront of innovation. Explore its real-world applications, challenges, and potential through these five essential questions.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Quantum (ORG), sci-fi (ORG), five (CARDINAL)</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/high-frequency-solutions-how-to-manage-burgeoning-data-traffic-on-a-finite-rf-spectrum-0001</t>
+          <t>https://www.rfglobalnet.com/doc/quantum-computing-top-questions-answered-0001</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Trends In Wind Power Generation</t>
+          <t>How To Manage Burgeoning Data Traffic On A Finite RF Spectrum</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>6/4/2024</t>
+          <t>6/5/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Explore the latest trends in wind power generation, focusing on advancements in turbine capacity, offshore installations, and the evolving requirements for power electronics to meet surging global demand.</t>
+          <t>Explore strategies and innovations to unlock higher-frequency bandwidths, which are crucial for sustaining technological advancement and meeting the escalating demands of our connected future.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/trends-in-wind-power-generation-0001</t>
+          <t>https://www.rfglobalnet.com/doc/high-frequency-solutions-how-to-manage-burgeoning-data-traffic-on-a-finite-rf-spectrum-0001</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>The Future Of Wi-Fi HaLow IP Cameras</t>
+          <t xml:space="preserve"> Trends In Wind Power Generation</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1004,20 +1008,20 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Wi-Fi HaLow offers extended range, better obstacle penetration, lower power consumption, and enhanced security for home security cameras, addressing limitations of traditional Wi-Fi and enabling robust, long-range connectivity.</t>
+          <t>Explore the latest trends in wind power generation, focusing on advancements in turbine capacity, offshore installations, and the evolving requirements for power electronics to meet surging global demand.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-future-of-wi-fi-halow-ip-cameras-0001</t>
+          <t>https://www.rfglobalnet.com/doc/trends-in-wind-power-generation-0001</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>State Of Open-Source DPI - Challenges, Opportunities And Alternatives</t>
+          <t>The Future Of Wi-Fi HaLow IP Cameras</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1027,278 +1031,274 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Learn about open-source Deep Packet Inspection (DPI) technology, its advantages and constraints, and the transition to commercial DPI. Learn about DPI engines and the need for commercial DPI solutions.</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Deep Packet Inspection (DPI (ORG)</t>
-        </is>
-      </c>
+          <t>Wi-Fi HaLow offers extended range, better obstacle penetration, lower power consumption, and enhanced security for home security cameras, addressing limitations of traditional Wi-Fi and enabling robust, long-range connectivity.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/state-of-open-source-dpi-challenges-opportunities-and-alternatives-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-future-of-wi-fi-halow-ip-cameras-0001</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Fundamental Capacitor Functions In The World Of Electronics</t>
+          <t>State Of Open-Source DPI - Challenges, Opportunities And Alternatives</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6/3/2024</t>
+          <t>6/4/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Understanding the versatile roles of capacitors is crucial in electronics, from power systems to RF applications. Learn their universal functions and applications.</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>Learn about open-source Deep Packet Inspection (DPI) technology, its advantages and constraints, and the transition to commercial DPI. Learn about DPI engines and the need for commercial DPI solutions.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Deep Packet Inspection (DPI (ORG)</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/fundamental-capacitor-functions-in-the-world-of-electronics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/state-of-open-source-dpi-challenges-opportunities-and-alternatives-0001</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Technical Report: Simulation Of Plasma Materials In XFdtd</t>
+          <t>Fundamental Capacitor Functions In The World Of Electronics</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/31/2024</t>
+          <t>6/3/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>This paper discusses the FDTD method to simulate the behavior of plasma materials using Remcom’s XFdtd 3D EM Simulation Software and presents validation in one and three dimensions.</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>FDTD (ORG), Remcom (ORG), XFdtd (ORG), one (CARDINAL), three (CARDINAL)</t>
-        </is>
-      </c>
+          <t>Understanding the versatile roles of capacitors is crucial in electronics, from power systems to RF applications. Learn their universal functions and applications.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/technical-report-simulation-of-plasma-materials-in-xfdtd-0001</t>
+          <t>https://www.rfglobalnet.com/doc/fundamental-capacitor-functions-in-the-world-of-electronics-0001</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Characterizing Parasitic Components In Power Converters</t>
+          <t>Technical Report: Simulation Of Plasma Materials In XFdtd</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/24/2024</t>
+          <t>5/31/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>With the rise of wide-bandgap semiconductors like GaN and SiC, characterizing parasitic components in power converters is crucial for maintaining efficiency and preventing performance issues.</t>
+          <t>This paper discusses the FDTD method to simulate the behavior of plasma materials using Remcom’s XFdtd 3D EM Simulation Software and presents validation in one and three dimensions.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>GaN (GPE), SiC (ORG)</t>
+          <t>FDTD (ORG), Remcom (ORG), XFdtd (ORG), one (CARDINAL), three (CARDINAL)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/characterizing-parasitic-components-in-power-converters-0001</t>
+          <t>https://www.rfglobalnet.com/doc/technical-report-simulation-of-plasma-materials-in-xfdtd-0001</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>New Microwave Products Expand Your Capabilities</t>
+          <t>Characterizing Parasitic Components In Power Converters</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/20/2024</t>
+          <t>5/24/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Explore a range of new microwave products, including dual-band filters, bandpass filters, couplers, and wideband assemblies, catering to diverse applications with compact designs and expanded frequency options.</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
+          <t>With the rise of wide-bandgap semiconductors like GaN and SiC, characterizing parasitic components in power converters is crucial for maintaining efficiency and preventing performance issues.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>GaN (GPE), SiC (ORG)</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/new-microwave-products-expand-your-capabilities-0001</t>
+          <t>https://www.rfglobalnet.com/doc/characterizing-parasitic-components-in-power-converters-0001</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>'Connected Car For Dummies' Reveals Cutting-Edge Innovations Shaping The Future Of Driving</t>
+          <t>New Microwave Products Expand Your Capabilities</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/17/2024</t>
+          <t>5/20/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Dive into excerpts from "Connected Car For Dummies, 2nd Edition," which explore the innovations—like lane assist, auto braking, and semi-autonomous driving—transforming the automotive industry.</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Connected Car For Dummies (WORK_OF_ART), 2nd Edition (PRODUCT)</t>
-        </is>
-      </c>
+          <t>Explore a range of new microwave products, including dual-band filters, bandpass filters, couplers, and wideband assemblies, catering to diverse applications with compact designs and expanded frequency options.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/connected-car-for-dummies-reveals-cutting-edge-innovations-shaping-the-future-of-driving-0001</t>
+          <t>https://www.rfglobalnet.com/doc/new-microwave-products-expand-your-capabilities-0001</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Green IT Strategies Set New Standards for Computing</t>
+          <t>'Connected Car For Dummies' Reveals Cutting-Edge Innovations Shaping The Future Of Driving</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/16/2024</t>
+          <t>5/17/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Mounting climate concerns affect virtually every industry. The tech sector is no exception, especially given the energy-reliant industry’s role in rising emissions and waste. Many organizations are looking to embrace green IT strategies amid this trend.</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
+          <t>Dive into excerpts from "Connected Car For Dummies, 2nd Edition," which explore the innovations—like lane assist, auto braking, and semi-autonomous driving—transforming the automotive industry.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Connected Car For Dummies (WORK_OF_ART), 2nd Edition (PRODUCT)</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/green-it-strategies-set-new-standards-for-computing-0001</t>
+          <t>https://www.rfglobalnet.com/doc/connected-car-for-dummies-reveals-cutting-edge-innovations-shaping-the-future-of-driving-0001</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Exploring The Capacitor Technologies Needed In Electric Vehicles</t>
+          <t>Green IT Strategies Set New Standards for Computing</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/10/2024</t>
+          <t>5/16/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Dive into the intricacies of capacitor technologies crucial for electric vehicles, deciphering their roles across traction inverters, onboard chargers, and DC/DC converters.</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>DC/DC (ORG)</t>
-        </is>
-      </c>
+          <t>Mounting climate concerns affect virtually every industry. The tech sector is no exception, especially given the energy-reliant industry’s role in rising emissions and waste. Many organizations are looking to embrace green IT strategies amid this trend.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/exploring-the-capacitor-technologies-needed-in-electric-vehicles-0001</t>
+          <t>https://www.rfglobalnet.com/doc/green-it-strategies-set-new-standards-for-computing-0001</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Enabling Powerful CCDF Statistical Analysis With RF Peak Power Sensors</t>
+          <t>Exploring The Capacitor Technologies Needed In Electric Vehicles</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/8/2024</t>
+          <t>5/10/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Learn how RF peak power sensors facilitate CCDF statistical analysis, essential for optimizing advanced wireless systems like 5G, tackling crest factor measurement challenges, and amplifier non-linearity.</t>
+          <t>Dive into the intricacies of capacitor technologies crucial for electric vehicles, deciphering their roles across traction inverters, onboard chargers, and DC/DC converters.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>RF (ORG), 5G (PERSON)</t>
+          <t>DC/DC (ORG)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/rf-peak-power-sensors-enable-powerful-ccdf-statistical-analysis-for-advanced-wireless-systems-0001</t>
+          <t>https://www.rfglobalnet.com/doc/exploring-the-capacitor-technologies-needed-in-electric-vehicles-0001</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>The Influence Of Phase In Filters For Radar</t>
+          <t>Enabling Powerful CCDF Statistical Analysis With RF Peak Power Sensors</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/6/2024</t>
+          <t>5/8/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Explore the crucial role of phase in radar filter performance, from maintaining beam position to achieving accurate measurements across temperature variations and frequency shifts.</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
+          <t>Learn how RF peak power sensors facilitate CCDF statistical analysis, essential for optimizing advanced wireless systems like 5G, tackling crest factor measurement challenges, and amplifier non-linearity.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>RF (ORG), 5G (PERSON)</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-influence-of-phase-in-filters-for-radar-0001</t>
+          <t>https://www.rfglobalnet.com/doc/rf-peak-power-sensors-enable-powerful-ccdf-statistical-analysis-for-advanced-wireless-systems-0001</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>The Power Of Connectivity: Smart Home Insights</t>
+          <t>The Influence Of Phase In Filters For Radar</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/30/2024</t>
+          <t>5/6/2024</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Discover how Matter™ standard revolutionizes IoT compatibility and fosters seamless collaboration among smart devices, unlocking a unified, intuitive, and truly connected living environment.</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>IoT (ORG)</t>
-        </is>
-      </c>
+          <t>Explore the crucial role of phase in radar filter performance, from maintaining beam position to achieving accurate measurements across temperature variations and frequency shifts.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-power-of-connectivity-smart-home-insights-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-influence-of-phase-in-filters-for-radar-0001</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Improving Range With ConcurrentConnect Antenna Diversity</t>
+          <t>The Power Of Connectivity: Smart Home Insights</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1308,47 +1308,47 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Learn about the performance benefits of antenna diversity technology for low-power wireless controllers and its ease of deployment in connected devices operating in constrained environments.</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
+          <t>Discover how Matter™ standard revolutionizes IoT compatibility and fosters seamless collaboration among smart devices, unlocking a unified, intuitive, and truly connected living environment.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>IoT (ORG)</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/improving-range-with-concurrentconnect-antenna-diversity-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-power-of-connectivity-smart-home-insights-0001</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Examining The Latest Electric Vehicle Technology Trends</t>
+          <t>Improving Range With ConcurrentConnect Antenna Diversity</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/22/2024</t>
+          <t>4/30/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Stay ahead in the world of electric vehicle (EV) development with insights into three key trends: wide band gap semiconductors, in-vehicle system integration, and the evolving EV charging ecosystem.</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>EV (ORG), three (CARDINAL), EV (ORG)</t>
-        </is>
-      </c>
+          <t>Learn about the performance benefits of antenna diversity technology for low-power wireless controllers and its ease of deployment in connected devices operating in constrained environments.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/examining-the-latest-electric-vehicle-technology-trends-0001</t>
+          <t>https://www.rfglobalnet.com/doc/improving-range-with-concurrentconnect-antenna-diversity-0001</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Thermal Design For Semiconductors And High Power GaN</t>
+          <t>Examining The Latest Electric Vehicle Technology Trends</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1358,74 +1358,74 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Navigating the complexities of thermal design is crucial for reliability in high-power applications. Let's delve into key considerations, focusing on gallium nitride (GaN) devices.</t>
+          <t>Stay ahead in the world of electric vehicle (EV) development with insights into three key trends: wide band gap semiconductors, in-vehicle system integration, and the evolving EV charging ecosystem.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>GaN (ORG)</t>
+          <t>EV (ORG), three (CARDINAL), EV (ORG)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/thermal-design-for-semiconductors-and-high-power-gan-0001</t>
+          <t>https://www.rfglobalnet.com/doc/examining-the-latest-electric-vehicle-technology-trends-0001</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mastering Phase Noise Measurement In Oscillator Production</t>
+          <t>Thermal Design For Semiconductors And High Power GaN</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/12/2024</t>
+          <t>4/22/2024</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Manufacturers producing products containing oscillators must understand how to measure phase noise and reduce it if necessary. Failing to take phase noise measurements as a part of the quality control process can reduce the item’s performance and reliability. Phase noise occurs when the phase of an oscillator’s output signal in the frequency domain fluctuates. Why does that matter, and which phase-noise measurement techniques should people use?</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr"/>
+          <t>Navigating the complexities of thermal design is crucial for reliability in high-power applications. Let's delve into key considerations, focusing on gallium nitride (GaN) devices.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>GaN (ORG)</t>
+        </is>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/mastering-phase-noise-measurement-in-oscillator-production-0001</t>
+          <t>https://www.rfglobalnet.com/doc/thermal-design-for-semiconductors-and-high-power-gan-0001</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Machined And Plated Solutions For Passive Electronic Components</t>
+          <t>Mastering Phase Noise Measurement In Oscillator Production</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/11/2024</t>
+          <t>4/12/2024</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Discover how an in-house tooling and fabrication shop ensures custom RF components meet exact specifications for manufacturing efficiency and consistency.</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>RF (ORG)</t>
-        </is>
-      </c>
+          <t>Manufacturers producing products containing oscillators must understand how to measure phase noise and reduce it if necessary. Failing to take phase noise measurements as a part of the quality control process can reduce the item’s performance and reliability. Phase noise occurs when the phase of an oscillator’s output signal in the frequency domain fluctuates. Why does that matter, and which phase-noise measurement techniques should people use?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/machined-and-plated-solutions-for-passive-electronic-components-0001</t>
+          <t>https://www.rfglobalnet.com/doc/mastering-phase-noise-measurement-in-oscillator-production-0001</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Exploring Electronics Trends In Solar Power</t>
+          <t>Machined And Plated Solutions For Passive Electronic Components</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1435,101 +1435,101 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Driven by evolving CO₂ regulations, power electronics systems like PV and HVDC are shaping a sustainable future. Explore trends in PV, a key player in global energy, and its changing landscape.</t>
+          <t>Discover how an in-house tooling and fabrication shop ensures custom RF components meet exact specifications for manufacturing efficiency and consistency.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>PV (FAC), HVDC (ORG), PV (FAC)</t>
+          <t>RF (ORG)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/exploring-electronics-trends-in-solar-power-0001</t>
+          <t>https://www.rfglobalnet.com/doc/machined-and-plated-solutions-for-passive-electronic-components-0001</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Filters In Radar Receivers</t>
+          <t>Exploring Electronics Trends In Solar Power</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/8/2024</t>
+          <t>4/11/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Explore how filters in radar receivers tackle signal problems, from band selection to interference removal, as technology evolves toward direct sampling and digital beamforming in radar systems.</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
+          <t>Driven by evolving CO₂ regulations, power electronics systems like PV and HVDC are shaping a sustainable future. Explore trends in PV, a key player in global energy, and its changing landscape.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>PV (FAC), HVDC (ORG), PV (FAC)</t>
+        </is>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/filters-in-radar-receivers-0001</t>
+          <t>https://www.rfglobalnet.com/doc/exploring-electronics-trends-in-solar-power-0001</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>What's New With UAVs In An Uncrewed World</t>
+          <t>Filters In Radar Receivers</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>4/8/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>From SeaGuardian to Stingray, discover how next-gen UAVs redefine missions with extended range, autonomy, and groundbreaking applications.</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>SeaGuardian (ORG), Stingray (ORG)</t>
-        </is>
-      </c>
+          <t>Explore how filters in radar receivers tackle signal problems, from band selection to interference removal, as technology evolves toward direct sampling and digital beamforming in radar systems.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/what-s-new-with-uavs-in-an-uncrewed-world-0001</t>
+          <t>https://www.rfglobalnet.com/doc/filters-in-radar-receivers-0001</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>New, 3-Cell Supercapacitors Support Significant Jump In Energy Storage</t>
+          <t>What's New With UAVs In An Uncrewed World</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3/25/2024</t>
+          <t>4/5/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>New 3-cell supercapacitors offer up to 9.0 WVDC, with high power density, low self-discharge, and over 500,000 charge cycles. Ideal for various energy storage applications.</t>
+          <t>From SeaGuardian to Stingray, discover how next-gen UAVs redefine missions with extended range, autonomy, and groundbreaking applications.</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3 (CARDINAL), over 500,000 (CARDINAL)</t>
+          <t>SeaGuardian (ORG), Stingray (ORG)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/new-cell-supercapacitors-support-significant-jump-in-energy-storage-0001</t>
+          <t>https://www.rfglobalnet.com/doc/what-s-new-with-uavs-in-an-uncrewed-world-0001</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>The Advantages Of The Qorvo SiC FET Vs SiC MOSFETs</t>
+          <t>New, 3-Cell Supercapacitors Support Significant Jump In Energy Storage</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1539,51 +1539,51 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>As SiC gains momentum, Qorvo's innovative 'cascode' FET device sets a new standard with enhanced efficiency, smaller size, and design flexibility.</t>
+          <t>New 3-cell supercapacitors offer up to 9.0 WVDC, with high power density, low self-discharge, and over 500,000 charge cycles. Ideal for various energy storage applications.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Qorvo (PERSON), FET (ORG)</t>
+          <t>3 (CARDINAL), over 500,000 (CARDINAL)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-advantages-of-the-qorvo-sic-fet-vs-sic-mosfets-0001</t>
+          <t>https://www.rfglobalnet.com/doc/new-cell-supercapacitors-support-significant-jump-in-energy-storage-0001</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>7 Unforgettable Ways IoT Is Reinventing Product Design</t>
+          <t>The Advantages Of The Qorvo SiC FET Vs SiC MOSFETs</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3/21/2024</t>
+          <t>3/25/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The Internet of Things (IoT) has changed how the world operates on several fronts. One of the most impactful of these shifts for businesses is how the IoT and product design have influenced one another over the past few years.</t>
+          <t>As SiC gains momentum, Qorvo's innovative 'cascode' FET device sets a new standard with enhanced efficiency, smaller size, and design flexibility.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>One (CARDINAL), IoT (ORG), the past few years (DATE)</t>
+          <t>Qorvo (PERSON), FET (ORG)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/unforgettable-ways-iot-is-reinventing-product-design-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-advantages-of-the-qorvo-sic-fet-vs-sic-mosfets-0001</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Pioneering A New Era Of Efficient And Sustainable Broadcast Distribution</t>
+          <t>7 Unforgettable Ways IoT Is Reinventing Product Design</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1593,151 +1593,155 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>In an era demanding sustainability and cost-effectiveness, the TE1 transmitter pioneers a 40% reduction in power consumption, shaping a greener broadcasting landscape.</t>
+          <t>The Internet of Things (IoT) has changed how the world operates on several fronts. One of the most impactful of these shifts for businesses is how the IoT and product design have influenced one another over the past few years.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>TE1 (ORG), 40% (PERCENT)</t>
+          <t>One (CARDINAL), IoT (ORG), the past few years (DATE)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/pioneering-a-new-era-of-efficient-and-sustainable-broadcast-distribution-0001</t>
+          <t>https://www.rfglobalnet.com/doc/unforgettable-ways-iot-is-reinventing-product-design-0001</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Inductors, Air Core Inductors And Baluns</t>
+          <t>Pioneering A New Era Of Efficient And Sustainable Broadcast Distribution</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>3/15/2024</t>
+          <t>3/21/2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Explore the fundamentals of inductors, from their role in circuits to the advantages of air core types. Plus, unravel the significance of baluns in maintaining signal balance.</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr"/>
+          <t>In an era demanding sustainability and cost-effectiveness, the TE1 transmitter pioneers a 40% reduction in power consumption, shaping a greener broadcasting landscape.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>TE1 (ORG), 40% (PERCENT)</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/inductors-air-core-inductors-and-baluns-0001</t>
+          <t>https://www.rfglobalnet.com/doc/pioneering-a-new-era-of-efficient-and-sustainable-broadcast-distribution-0001</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Switch Filter Banks For Agile RF Receiver Design In Radar</t>
+          <t>Inductors, Air Core Inductors And Baluns</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>3/8/2024</t>
+          <t>3/15/2024</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>In this installment of our RF Components for Radar series, we delve into switch filter banks, which are essential for optimizing radar performance in congested spectra.</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Radar (PRODUCT)</t>
-        </is>
-      </c>
+          <t>Explore the fundamentals of inductors, from their role in circuits to the advantages of air core types. Plus, unravel the significance of baluns in maintaining signal balance.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/switch-filter-banks-for-agile-rf-receiver-design-in-radar-0001</t>
+          <t>https://www.rfglobalnet.com/doc/inductors-air-core-inductors-and-baluns-0001</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Examining Trends In Power Electronics</t>
+          <t>Switch Filter Banks For Agile RF Receiver Design In Radar</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3/7/2024</t>
+          <t>3/8/2024</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Navigating the dynamic landscape of power electronics requires a keen eye on evolving trends. Explore four key developments shaping the industry and innovative solutions that help you stay ahead.</t>
+          <t>In this installment of our RF Components for Radar series, we delve into switch filter banks, which are essential for optimizing radar performance in congested spectra.</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>four (CARDINAL)</t>
+          <t>Radar (PRODUCT)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/examining-trends-in-power-electronics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/switch-filter-banks-for-agile-rf-receiver-design-in-radar-0001</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>RF Components For Radar: Overview And Trends</t>
+          <t>Examining Trends In Power Electronics</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3/4/2024</t>
+          <t>3/7/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Radar systems play a crucial role in detecting and locating objects. Explore the key functional components and technological evolution, from duplexing to digital-array radar, in this overview.</t>
+          <t>Navigating the dynamic landscape of power electronics requires a keen eye on evolving trends. Explore four key developments shaping the industry and innovative solutions that help you stay ahead.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Radar (PRODUCT)</t>
+          <t>four (CARDINAL)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/rf-components-for-radar-overview-and-trends-0001</t>
+          <t>https://www.rfglobalnet.com/doc/examining-trends-in-power-electronics-0001</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Integrating X-band Radar For Next-Level Detection And Imaging</t>
+          <t>RF Components For Radar: Overview And Trends</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2/26/2024</t>
+          <t>3/4/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Explore the evolution and integration challenges of X-band radar, a pivotal technology boasting superior resolution and compactness, shaping modern radar solutions.</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
+          <t>Radar systems play a crucial role in detecting and locating objects. Explore the key functional components and technological evolution, from duplexing to digital-array radar, in this overview.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Radar (PRODUCT)</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-future-is-here-integrating-x-band-radar-for-next-level-detection-and-imaging-0001</t>
+          <t>https://www.rfglobalnet.com/doc/rf-components-for-radar-overview-and-trends-0001</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Force Sensing Solutions Pave The Way For Automotive Evolution</t>
+          <t>Integrating X-band Radar For Next-Level Detection And Imaging</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1747,20 +1751,20 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Amidst a wave of technological advancements, automobiles are undergoing a monumental evolution, integrating smart surfaces and sensing solutions to redefine the in-cabin experience.</t>
+          <t>Explore the evolution and integration challenges of X-band radar, a pivotal technology boasting superior resolution and compactness, shaping modern radar solutions.</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/beyond-buttons-force-sensing-solutions-pave-the-way-for-automotive-evolution-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-future-is-here-integrating-x-band-radar-for-next-level-detection-and-imaging-0001</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Shedding More Light On Ultra-Wideband</t>
+          <t>Force Sensing Solutions Pave The Way For Automotive Evolution</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1770,209 +1774,205 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Discover how Ultra-Wideband (UWB) technology is revolutionizing manufacturing by providing unparalleled precision in locating products and optimizing processes for enhanced efficiency and safety.</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Ultra-Wideband (NORP)</t>
-        </is>
-      </c>
+          <t>Amidst a wave of technological advancements, automobiles are undergoing a monumental evolution, integrating smart surfaces and sensing solutions to redefine the in-cabin experience.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/ultra-wideband-case-study-shedding-more-light-on-uwb-0001</t>
+          <t>https://www.rfglobalnet.com/doc/beyond-buttons-force-sensing-solutions-pave-the-way-for-automotive-evolution-0001</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>How To Size A Snubber Capacitor For Your Power Supply</t>
+          <t>Shedding More Light On Ultra-Wideband</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2/15/2024</t>
+          <t>2/26/2024</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Explore snubber derivation for a simple switching circuit, a helpful exercise in understanding how these switches impact snubber capacitor sizing.</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
+          <t>Discover how Ultra-Wideband (UWB) technology is revolutionizing manufacturing by providing unparalleled precision in locating products and optimizing processes for enhanced efficiency and safety.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Ultra-Wideband (NORP)</t>
+        </is>
+      </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/how-to-size-a-snubber-capacitor-for-your-power-supply-0001</t>
+          <t>https://www.rfglobalnet.com/doc/ultra-wideband-case-study-shedding-more-light-on-uwb-0001</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Large-Scale, 24/7 Mobile Quality Monitoring And Service Level Verification</t>
+          <t>How To Size A Snubber Capacitor For Your Power Supply</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1/27/2024</t>
+          <t>2/15/2024</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Learn how CERN, the European Organization for Nuclear Research, created a reliable, cost-efficient, and fully compliant monitoring system for SLA verification with Android Probe and MNT solutions.</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>CERN (GPE), the European Organization for Nuclear Research (ORG), Android Probe (PERSON), MNT (PERSON)</t>
-        </is>
-      </c>
+          <t>Explore snubber derivation for a simple switching circuit, a helpful exercise in understanding how these switches impact snubber capacitor sizing.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/large-scale-mobile-quality-monitoring-and-service-level-verification-0001</t>
+          <t>https://www.rfglobalnet.com/doc/how-to-size-a-snubber-capacitor-for-your-power-supply-0001</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Focusing On Ways To Better Support You In 2024 And Beyond</t>
+          <t>Large-Scale, 24/7 Mobile Quality Monitoring And Service Level Verification</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1/24/2024</t>
+          <t>1/27/2024</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Knowles President Chris Dugann reflects on an exciting year, including the acquisition of Cornell Dubilier, while emphasizing a commitment to supporting core markets with innovative solutions.</t>
+          <t>Learn how CERN, the European Organization for Nuclear Research, created a reliable, cost-efficient, and fully compliant monitoring system for SLA verification with Android Probe and MNT solutions.</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Chris Dugann (PERSON), an exciting year (DATE), Cornell Dubilier (ORG)</t>
+          <t>CERN (GPE), the European Organization for Nuclear Research (ORG), Android Probe (PERSON), MNT (PERSON)</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/focusing-on-ways-to-better-support-you-in-and-beyond-0001</t>
+          <t>https://www.rfglobalnet.com/doc/large-scale-mobile-quality-monitoring-and-service-level-verification-0001</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Exploring Automated Frequency Coordination (AFC) In The Wi-Fi 6GHz Realm</t>
+          <t>Focusing On Ways To Better Support You In 2024 And Beyond</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1/22/2024</t>
+          <t>1/24/2024</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Examine the implications of Wi-Fi 6E/7 tri-band coexistence measures and how the FCC is working to ensure a harmonious coexistence between Wi-Fi and other licensed and unlicensed radios in the US.</t>
+          <t>Knowles President Chris Dugann reflects on an exciting year, including the acquisition of Cornell Dubilier, while emphasizing a commitment to supporting core markets with innovative solutions.</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6E/7 (CARDINAL), FCC (ORG), US (GPE)</t>
+          <t>Chris Dugann (PERSON), an exciting year (DATE), Cornell Dubilier (ORG)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/exploring-automated-frequency-coordination-afc-in-the-wi-fi-ghz-realm-0001</t>
+          <t>https://www.rfglobalnet.com/doc/focusing-on-ways-to-better-support-you-in-and-beyond-0001</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Quantum-Enabled Radar Research: Finding The Right Solution</t>
+          <t>Exploring Automated Frequency Coordination (AFC) In The Wi-Fi 6GHz Realm</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1/16/2024</t>
+          <t>1/22/2024</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Examine how high-precision measurement of oscillators helped UK Quantum Technology Hub research to develop high-precision radar for detecting small objects such as drones and birds.</t>
+          <t>Examine the implications of Wi-Fi 6E/7 tri-band coexistence measures and how the FCC is working to ensure a harmonious coexistence between Wi-Fi and other licensed and unlicensed radios in the US.</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>UK Quantum Technology Hub (ORG)</t>
+          <t>6E/7 (CARDINAL), FCC (ORG), US (GPE)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/quantum-enabled-radar-research-finding-the-right-solution-for-the-university-of-birmingham-0001</t>
+          <t>https://www.rfglobalnet.com/doc/exploring-automated-frequency-coordination-afc-in-the-wi-fi-ghz-realm-0001</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>The Roles Of Capacitors In EV Traction Inverter Topologies</t>
+          <t>Quantum-Enabled Radar Research: Finding The Right Solution</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>1/5/2024</t>
+          <t>1/16/2024</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Choosing the right capacitor is crucial for your EV's performance, reliability, and safety. Understand the capacitor types and functions to make an informed decision for your EV traction inverter.</t>
+          <t>Examine how high-precision measurement of oscillators helped UK Quantum Technology Hub research to develop high-precision radar for detecting small objects such as drones and birds.</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>EV (ORG)</t>
+          <t>UK Quantum Technology Hub (ORG)</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-roles-of-capacitors-in-ev-traction-inverter-topologies-0001</t>
+          <t>https://www.rfglobalnet.com/doc/quantum-enabled-radar-research-finding-the-right-solution-for-the-university-of-birmingham-0001</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Understanding Equivalent Series Resistance And Q Factor</t>
+          <t>The Roles Of Capacitors In EV Traction Inverter Topologies</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1/3/2024</t>
+          <t>1/5/2024</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Equivalent Series Resistance (ESR) and Quality Factor (Q factor) are important figures in circuit design and understanding their value is key. Learn more about the roles of both factors.</t>
+          <t>Choosing the right capacitor is crucial for your EV's performance, reliability, and safety. Understand the capacitor types and functions to make an informed decision for your EV traction inverter.</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Equivalent Series Resistance (EVENT), ESR (ORG), Quality Factor (ORG)</t>
+          <t>EV (ORG)</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/today-s-rf-power-applications-require-understanding-equivalent-series-resistance-and-q-factor-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-roles-of-capacitors-in-ev-traction-inverter-topologies-0001</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Matter And Qorvo Provide Designers With A Game-Changing Boost</t>
+          <t>Understanding Equivalent Series Resistance And Q Factor</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1982,120 +1982,120 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Discover the impact of Matter's standardization and Qorvo's technological solutions in simplifying IoT devices and streamlining system design for a user-friendly and efficient smart home experience.</t>
+          <t>Equivalent Series Resistance (ESR) and Quality Factor (Q factor) are important figures in circuit design and understanding their value is key. Learn more about the roles of both factors.</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Matter (PERSON), Qorvo (GPE)</t>
+          <t>Equivalent Series Resistance (EVENT), ESR (ORG), Quality Factor (ORG)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/empowering-the-iot-ecosystem-matter-and-qorvo-provide-designers-with-a-game-changing-boost-0001</t>
+          <t>https://www.rfglobalnet.com/doc/today-s-rf-power-applications-require-understanding-equivalent-series-resistance-and-q-factor-0001</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>The Transition From Si To SiC In Power Electronics</t>
+          <t>Matter And Qorvo Provide Designers With A Game-Changing Boost</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1/2/2024</t>
+          <t>1/3/2024</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>There's been a shift in use from traditional silicon (Si) to silicon carbide (SiC) in power electronics. Explore the advantages that make SiC a breakthrough power electronic technology of the future.</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
+          <t>Discover the impact of Matter's standardization and Qorvo's technological solutions in simplifying IoT devices and streamlining system design for a user-friendly and efficient smart home experience.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Matter (PERSON), Qorvo (GPE)</t>
+        </is>
+      </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-transition-from-si-to-sic-in-power-electronics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/empowering-the-iot-ecosystem-matter-and-qorvo-provide-designers-with-a-game-changing-boost-0001</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Resonant Wireless Power Transfer In Implantable Medical Devices</t>
+          <t>The Transition From Si To SiC In Power Electronics</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>12/15/2023</t>
+          <t>1/2/2024</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Battery life and replacements can be problematic for implantable medical devices. Resonant wireless power transfer (RWPT) provides a safe and efficient solution.</t>
+          <t>There's been a shift in use from traditional silicon (Si) to silicon carbide (SiC) in power electronics. Explore the advantages that make SiC a breakthrough power electronic technology of the future.</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/resonant-wireless-power-transfer-in-implantable-medical-devices-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-transition-from-si-to-sic-in-power-electronics-0001</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Why Should Directed Energy Weapons Integrate An Additive White Gaussian Noise Source?</t>
+          <t>Resonant Wireless Power Transfer In Implantable Medical Devices</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>12/14/2023</t>
+          <t>12/15/2023</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Embedding a noise source into a laser weapon’s electronics can improve its effectiveness in neutralizing hostile targets. Explore the fundamentals of directed energy weapons with laser-based systems.</t>
+          <t>Battery life and replacements can be problematic for implantable medical devices. Resonant wireless power transfer (RWPT) provides a safe and efficient solution.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/why-should-directed-energy-weapons-integrate-an-additive-white-gaussian-noise-source-0001</t>
+          <t>https://www.rfglobalnet.com/doc/resonant-wireless-power-transfer-in-implantable-medical-devices-0001</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Gain Equalizer Basics</t>
+          <t>Why Should Directed Energy Weapons Integrate An Additive White Gaussian Noise Source?</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>11/30/2023</t>
+          <t>12/14/2023</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Discover how passive gain equalizers offer a solution to frequency response issues in RF amplifiers, providing advantages such as durability, flexibility, and low noise characteristics.</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>RF (ORG)</t>
-        </is>
-      </c>
+          <t>Embedding a noise source into a laser weapon’s electronics can improve its effectiveness in neutralizing hostile targets. Explore the fundamentals of directed energy weapons with laser-based systems.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/gain-equalizer-basics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/why-should-directed-energy-weapons-integrate-an-additive-white-gaussian-noise-source-0001</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>High Frequency (HF) Learning Center</t>
+          <t>Gain Equalizer Basics</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2105,20 +2105,24 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Explore an expansive learning center featuring videos, tutorials, white papers, brochures, application notes, quick links, and articles focused on High-Frequency Test and Measurement solutions.</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr"/>
+          <t>Discover how passive gain equalizers offer a solution to frequency response issues in RF amplifiers, providing advantages such as durability, flexibility, and low noise characteristics.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>RF (ORG)</t>
+        </is>
+      </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/high-frequency-hf-learning-center-0001</t>
+          <t>https://www.rfglobalnet.com/doc/gain-equalizer-basics-0001</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Contextualizing Q Factor</t>
+          <t>High Frequency (HF) Learning Center</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2128,74 +2132,74 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>An in-depth understanding of poles and zeros will improve your filter designs. Discover how open-source RF analysis tools can help you better understand how poles and zeros relate to Q factor.</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>zeros (CARDINAL), zeros (CARDINAL)</t>
-        </is>
-      </c>
+          <t>Explore an expansive learning center featuring videos, tutorials, white papers, brochures, application notes, quick links, and articles focused on High-Frequency Test and Measurement solutions.</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/contextualizing-q-factor-0001</t>
+          <t>https://www.rfglobalnet.com/doc/high-frequency-hf-learning-center-0001</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>The Role Of Resonant Capacitors In Power Electronics</t>
+          <t>Contextualizing Q Factor</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>11/28/2023</t>
+          <t>11/30/2023</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Explore the basic attributes of capacitors, like the ability to store electric charge and conduct higher-frequency AC currents, and the impact of extreme frequencies on their performance.</t>
+          <t>An in-depth understanding of poles and zeros will improve your filter designs. Discover how open-source RF analysis tools can help you better understand how poles and zeros relate to Q factor.</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>AC (ORG)</t>
+          <t>zeros (CARDINAL), zeros (CARDINAL)</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-role-of-resonant-capacitors-in-power-electronics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/contextualizing-q-factor-0001</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Non-Magnetic Trimmer Capacitors For In-Suite Or Portable MRI Machines</t>
+          <t>The Role Of Resonant Capacitors In Power Electronics</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>11/20/2023</t>
+          <t>11/28/2023</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Explore the types of non-magnetic surface-mount device (SMD) capacitors, including trimmer capacitors, that are crucial for maintaining reliability and optimal performance in POC MRI machines.</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
+          <t>Explore the basic attributes of capacitors, like the ability to store electric charge and conduct higher-frequency AC currents, and the impact of extreme frequencies on their performance.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>AC (ORG)</t>
+        </is>
+      </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/non-magnetic-trimmer-capacitors-for-in-suite-or-portable-mri-machines-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-role-of-resonant-capacitors-in-power-electronics-0001</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>What Are Bias Filter And Self-Bias Networks?</t>
+          <t>Non-Magnetic Trimmer Capacitors For In-Suite Or Portable MRI Machines</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2205,24 +2209,20 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Discover how bias filter and self-bias networks play a crucial role in ensuring RF amplifiers operate efficiently, maintain linearity, and minimize noise/interference.</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>RF (ORG)</t>
-        </is>
-      </c>
+          <t>Explore the types of non-magnetic surface-mount device (SMD) capacitors, including trimmer capacitors, that are crucial for maintaining reliability and optimal performance in POC MRI machines.</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/what-are-bias-filter-and-self-bias-networks-0001</t>
+          <t>https://www.rfglobalnet.com/doc/non-magnetic-trimmer-capacitors-for-in-suite-or-portable-mri-machines-0001</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Power Divider Basics</t>
+          <t>What Are Bias Filter And Self-Bias Networks?</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2232,120 +2232,124 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Power dividers are crucial in many areas, such as antenna systems, telecommunications, and signal processing. Know the different types and how to choose the right one for your application.</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr"/>
+          <t>Discover how bias filter and self-bias networks play a crucial role in ensuring RF amplifiers operate efficiently, maintain linearity, and minimize noise/interference.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>RF (ORG)</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/power-divider-basics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/what-are-bias-filter-and-self-bias-networks-0001</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Free And Fast Circuit Simulation For Mixed Analog And Digital</t>
+          <t>Power Divider Basics</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>11/13/2023</t>
+          <t>11/20/2023</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>QSPICE, an advanced SPICE simulator, redefines circuit analysis with groundbreaking mixed-signal capabilities. Its creators detail what makes it a game-changer for design engineers.</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>QSPICE (ORG), SPICE (ORG)</t>
-        </is>
-      </c>
+          <t>Power dividers are crucial in many areas, such as antenna systems, telecommunications, and signal processing. Know the different types and how to choose the right one for your application.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/a-much-spicier-spice-free-and-fast-circuit-simulation-for-mixed-analog-and-digital-0001</t>
+          <t>https://www.rfglobalnet.com/doc/power-divider-basics-0001</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>RedCap — A New Class Of 5G Devices</t>
+          <t>Free And Fast Circuit Simulation For Mixed Analog And Digital</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>11/3/2023</t>
+          <t>11/13/2023</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Discover the future of wireless with RedCap technology, part of 5G Release 17. RedCap enhances IoT device capabilities, enabling smaller, more efficient devices with extended battery life.</t>
+          <t>QSPICE, an advanced SPICE simulator, redefines circuit analysis with groundbreaking mixed-signal capabilities. Its creators detail what makes it a game-changer for design engineers.</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>RedCap (ORG), 5 (CARDINAL), IoT (EVENT)</t>
+          <t>QSPICE (ORG), SPICE (ORG)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/reduced-capabilities-redcap-a-new-class-of-g-devices-0001</t>
+          <t>https://www.rfglobalnet.com/doc/a-much-spicier-spice-free-and-fast-circuit-simulation-for-mixed-analog-and-digital-0001</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Interactivity Test: Testing Service Availability</t>
+          <t>RedCap — A New Class Of 5G Devices</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>11/2/2023</t>
+          <t>11/3/2023</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Discover insights from extensive testing of interactivity tests, an innovative approach that guarantees service availability, meeting the most stringent requirements, to revolutionize how we assess 5G.</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
+          <t>Discover the future of wireless with RedCap technology, part of 5G Release 17. RedCap enhances IoT device capabilities, enabling smaller, more efficient devices with extended battery life.</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>RedCap (ORG), 5 (CARDINAL), IoT (EVENT)</t>
+        </is>
+      </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/interactivity-test-testing-service-availability-0001</t>
+          <t>https://www.rfglobalnet.com/doc/reduced-capabilities-redcap-a-new-class-of-g-devices-0001</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Signal Generation Breakthroughs: Match-Corrected Measurements And De-Embedding</t>
+          <t>Interactivity Test: Testing Service Availability</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10/25/2023</t>
+          <t>11/2/2023</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Explore methods to improve wireless communication testing accuracy through vector network analyzers and reflectometers, addressing challenges such as impedance mismatch and frequency response errors.</t>
+          <t>Discover insights from extensive testing of interactivity tests, an innovative approach that guarantees service availability, meeting the most stringent requirements, to revolutionize how we assess 5G.</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/signal-generation-breakthroughs-match-corrected-measurements-and-de-embedding-0001</t>
+          <t>https://www.rfglobalnet.com/doc/interactivity-test-testing-service-availability-0001</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Closing The Gap: How Force Sensors Fuel Novel HMI Designs</t>
+          <t>Signal Generation Breakthroughs: Match-Corrected Measurements And De-Embedding</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2355,24 +2359,20 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Unlike traditional touch technologies, force-sensing MEMS devices redefine interfaces, eliminating the need for mechanical buttons and enabling gapless, waterproof designs.</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>MEMS (ORG)</t>
-        </is>
-      </c>
+          <t>Explore methods to improve wireless communication testing accuracy through vector network analyzers and reflectometers, addressing challenges such as impedance mismatch and frequency response errors.</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/closing-the-gap-how-force-sensors-fuel-novel-hmi-designs-0001</t>
+          <t>https://www.rfglobalnet.com/doc/signal-generation-breakthroughs-match-corrected-measurements-and-de-embedding-0001</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>True Time Delay: What It Is And How It Works</t>
+          <t>Closing The Gap: How Force Sensors Fuel Novel HMI Designs</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2382,24 +2382,24 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Discover how Phased Array Antennas adapt with wider bandwidths, true time delay, and AESA advancements, optimizing beam steering and improving signal quality.</t>
+          <t>Unlike traditional touch technologies, force-sensing MEMS devices redefine interfaces, eliminating the need for mechanical buttons and enabling gapless, waterproof designs.</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Array Antennas (PERSON), AESA (ORG)</t>
+          <t>MEMS (ORG)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/true-time-delay-what-it-is-and-how-it-works-0001</t>
+          <t>https://www.rfglobalnet.com/doc/closing-the-gap-how-force-sensors-fuel-novel-hmi-designs-0001</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Ray-Optical Modeling Of Wireless Coverage Enhancement Using Engineered Electromagnetic Surfaces</t>
+          <t>True Time Delay: What It Is And How It Works</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2409,182 +2409,186 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>In this paper, results are presented of propagation experiments conducted to verify the accuracy of a novel ray-optical scattering model for EES.</t>
+          <t>Discover how Phased Array Antennas adapt with wider bandwidths, true time delay, and AESA advancements, optimizing beam steering and improving signal quality.</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>EES (ORG)</t>
+          <t>Array Antennas (PERSON), AESA (ORG)</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/ray-optical-modeling-of-wireless-coverage-enhancement-using-engineered-electromagnetic-surfaces-experimental-verification-at-ghz-0001</t>
+          <t>https://www.rfglobalnet.com/doc/true-time-delay-what-it-is-and-how-it-works-0001</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>How GaN Semiconductors In Defense Power Supplies Affect Capacitor Selection</t>
+          <t>Ray-Optical Modeling Of Wireless Coverage Enhancement Using Engineered Electromagnetic Surfaces</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>10/23/2023</t>
+          <t>10/25/2023</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Explore the advantages of GaN semiconductors, including lower heat generation and a smaller footprint, and the crucial role ceramic capacitors play in optimizing these systems.</t>
+          <t>In this paper, results are presented of propagation experiments conducted to verify the accuracy of a novel ray-optical scattering model for EES.</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>GaN (NORP)</t>
+          <t>EES (ORG)</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/how-gallium-nitride-gan-semiconductors-in-defense-power-supplies-affect-capacitor-selection-0001</t>
+          <t>https://www.rfglobalnet.com/doc/ray-optical-modeling-of-wireless-coverage-enhancement-using-engineered-electromagnetic-surfaces-experimental-verification-at-ghz-0001</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>I'm Going As A Nobel Prize Winner For Halloween</t>
+          <t>How GaN Semiconductors In Defense Power Supplies Affect Capacitor Selection</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10/20/2023</t>
+          <t>10/23/2023</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>This year’s batch of Nobel Laureates all seem to be fine scientists, researchers, authors, and leaders who don’t seem to have anything to do with Halloween. But don’t worry, we found some past award winners who do!</t>
+          <t>Explore the advantages of GaN semiconductors, including lower heat generation and a smaller footprint, and the crucial role ceramic capacitors play in optimizing these systems.</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>year (DATE), Nobel Laureates (GPE), Halloween (DATE)</t>
+          <t>GaN (NORP)</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/i-m-going-as-a-nobel-prize-winner-for-halloween-0001</t>
+          <t>https://www.rfglobalnet.com/doc/how-gallium-nitride-gan-semiconductors-in-defense-power-supplies-affect-capacitor-selection-0001</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Smartphone Security In The Crosshairs: The Increasing Attractiveness Of Mobile Devices As Targets For Cyberattacks</t>
+          <t>I'm Going As A Nobel Prize Winner For Halloween</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10/10/2023</t>
+          <t>10/20/2023</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>According to the Group Speciale Mobile Association (GSMA), nine in ten consumers are concerned over smartphone data security and privacy. But how to ensure security in smartphones if they are such an attractive target? The answer is security can never be ensured, but we can make life much harder for hackers by following best practices when it comes to securing smartphones.</t>
+          <t>This year’s batch of Nobel Laureates all seem to be fine scientists, researchers, authors, and leaders who don’t seem to have anything to do with Halloween. But don’t worry, we found some past award winners who do!</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>the Group Speciale Mobile Association (ORG), nine (CARDINAL), ten (CARDINAL)</t>
+          <t>year (DATE), Nobel Laureates (GPE), Halloween (DATE)</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/smartphone-security-in-the-crosshairs-the-increasing-attractiveness-of-mobile-devices-as-targets-for-cyberattacks-0001</t>
+          <t>https://www.rfglobalnet.com/doc/i-m-going-as-a-nobel-prize-winner-for-halloween-0001</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>The Importance Of Safety Capacitors In Power Electronics</t>
+          <t>Smartphone Security In The Crosshairs: The Increasing Attractiveness Of Mobile Devices As Targets For Cyberattacks</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10/5/2023</t>
+          <t>10/10/2023</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Safety capacitors, such as Class-X and Class-Y capacitors, play a crucial role in mitigating transient voltages and EMI in electrical circuits, ensuring safe operation in various applications.</t>
+          <t>According to the Group Speciale Mobile Association (GSMA), nine in ten consumers are concerned over smartphone data security and privacy. But how to ensure security in smartphones if they are such an attractive target? The answer is security can never be ensured, but we can make life much harder for hackers by following best practices when it comes to securing smartphones.</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>EMI (ORG)</t>
+          <t>the Group Speciale Mobile Association (ORG), nine (CARDINAL), ten (CARDINAL)</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-importance-of-safety-capacitors-in-power-electronics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/smartphone-security-in-the-crosshairs-the-increasing-attractiveness-of-mobile-devices-as-targets-for-cyberattacks-0001</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>What Are DC Link Supporting Filters?</t>
+          <t>The Importance Of Safety Capacitors In Power Electronics</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>9/28/2023</t>
+          <t>10/5/2023</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Discover the role of capacitors in power electronics and learn about the benefits of adding ceramic capacitors to enhance performance and reliability on the DC link.</t>
+          <t>Safety capacitors, such as Class-X and Class-Y capacitors, play a crucial role in mitigating transient voltages and EMI in electrical circuits, ensuring safe operation in various applications.</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>DC (GPE)</t>
+          <t>EMI (ORG)</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/what-are-dc-link-supporting-filters-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-importance-of-safety-capacitors-in-power-electronics-0001</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Ubiquitous Connectivity Is The Future Of Wireless — Here's How Engineers Can Prepare</t>
+          <t>What Are DC Link Supporting Filters?</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>9/26/2023</t>
+          <t>9/28/2023</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>The main goal of wireless communications is to connect people regardless of their location, and achieving ubiquitous connectivity has become essential for modern wireless systems.</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr"/>
+          <t>Discover the role of capacitors in power electronics and learn about the benefits of adding ceramic capacitors to enhance performance and reliability on the DC link.</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>DC (GPE)</t>
+        </is>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/ubiquitous-connectivity-is-the-future-of-wireless-%E2%80%94-here%E2%80%99s-how-engineers-can-prepare-0001</t>
+          <t>https://www.rfglobalnet.com/doc/what-are-dc-link-supporting-filters-0001</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Understanding The Basics Of RF Signal Generation</t>
+          <t>Ubiquitous Connectivity Is The Future Of Wireless — Here's How Engineers Can Prepare</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2594,47 +2598,43 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>RF signal generators are a vital tool for testing and measuring. Despite advancements, their principles remain unchanged. We'll explore their structure and key metrics.</t>
+          <t>The main goal of wireless communications is to connect people regardless of their location, and achieving ubiquitous connectivity has become essential for modern wireless systems.</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/understanding-the-basics-of-rf-signal-generation-0001</t>
+          <t>https://www.rfglobalnet.com/doc/ubiquitous-connectivity-is-the-future-of-wireless-%E2%80%94-here%E2%80%99s-how-engineers-can-prepare-0001</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Power Solutions For Phased Radar</t>
+          <t>Understanding The Basics Of RF Signal Generation</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>9/25/2023</t>
+          <t>9/26/2023</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Gallium Nitride (GaN) technology, with its higher power, wider bandwidth, and high breakdown voltage, has evolved and found a niche in radar systems, with PMICs simplifying its operational requirements.</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Gallium Nitride (PERSON), GaN (GPE)</t>
-        </is>
-      </c>
+          <t>RF signal generators are a vital tool for testing and measuring. Despite advancements, their principles remain unchanged. We'll explore their structure and key metrics.</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/power-solutions-for-phased-radar-0001</t>
+          <t>https://www.rfglobalnet.com/doc/understanding-the-basics-of-rf-signal-generation-0001</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Wide Bandgap FETs Make Regulating High Voltage Simple</t>
+          <t>Power Solutions For Phased Radar</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2644,70 +2644,74 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Wide bandgap FETs simplify high-voltage regulation, offering improved performance and eliminating the need for a negative rail in comparison to older transistor-based designs.</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr"/>
+          <t>Gallium Nitride (GaN) technology, with its higher power, wider bandwidth, and high breakdown voltage, has evolved and found a niche in radar systems, with PMICs simplifying its operational requirements.</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Gallium Nitride (PERSON), GaN (GPE)</t>
+        </is>
+      </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/wide-bandgap-fets-make-regulating-high-voltage-simple-0001</t>
+          <t>https://www.rfglobalnet.com/doc/power-solutions-for-phased-radar-0001</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Understanding The Crucial Role of Snubber Capacitors In Power Electronics</t>
+          <t>Wide Bandgap FETs Make Regulating High Voltage Simple</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>9/22/2023</t>
+          <t>9/25/2023</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>A snubber capacitor safeguards electronics from voltage spikes during high-current switching, improving efficiency and reducing EMI.</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>EMI (ORG)</t>
-        </is>
-      </c>
+          <t>Wide bandgap FETs simplify high-voltage regulation, offering improved performance and eliminating the need for a negative rail in comparison to older transistor-based designs.</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/understanding-the-crucial-role-of-snubber-capacitors-in-power-electronics-0001</t>
+          <t>https://www.rfglobalnet.com/doc/wide-bandgap-fets-make-regulating-high-voltage-simple-0001</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Case Study: Secure Electronic Warfare Systems</t>
+          <t>Understanding The Crucial Role of Snubber Capacitors In Power Electronics</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9/20/2023</t>
+          <t>9/22/2023</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>The most advanced microelectronics technology is critical for the aerospace and defense industry. For this customer, that meant state-of-the-art heterogeneous processing.</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
+          <t>A snubber capacitor safeguards electronics from voltage spikes during high-current switching, improving efficiency and reducing EMI.</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>EMI (ORG)</t>
+        </is>
+      </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/case-study-secure-electronic-warfare-systems-0001</t>
+          <t>https://www.rfglobalnet.com/doc/understanding-the-crucial-role-of-snubber-capacitors-in-power-electronics-0001</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>What Are Bootstrap Capacitors?</t>
+          <t>Case Study: Secure Electronic Warfare Systems</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2717,20 +2721,20 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Components like bootstrap capacitors are increasingly vital for efficiently managing electrical energy in applications such as electric vehicles, renewable energy systems, and consumer electronics.</t>
+          <t>The most advanced microelectronics technology is critical for the aerospace and defense industry. For this customer, that meant state-of-the-art heterogeneous processing.</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/what-are-bootstrap-capacitors-0001</t>
+          <t>https://www.rfglobalnet.com/doc/case-study-secure-electronic-warfare-systems-0001</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>High Q Capacitors – Roles And Specifications</t>
+          <t>What Are Bootstrap Capacitors?</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2740,101 +2744,97 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>The Q factor measures a capacitor's efficiency in storing and dissipating energy at a specific frequency, with a high Q indicating low energy loss and suitability for low-power, stable applications.</t>
+          <t>Components like bootstrap capacitors are increasingly vital for efficiently managing electrical energy in applications such as electric vehicles, renewable energy systems, and consumer electronics.</t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/high-q-capacitors-roles-and-specifications-0001</t>
+          <t>https://www.rfglobalnet.com/doc/what-are-bootstrap-capacitors-0001</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Delivering Big Switching Power In A Small Package With SiC FETs</t>
+          <t>High Q Capacitors – Roles And Specifications</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>9/12/2023</t>
+          <t>9/20/2023</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>New SiC and GaN semiconductor switches offer better efficiency and smaller size than silicon-based parts. Qorvo's 750V SiC-FET in a compact TOLL package can greatly benefit your design.</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>GaN (ORG), Qorvo (GPE)</t>
-        </is>
-      </c>
+          <t>The Q factor measures a capacitor's efficiency in storing and dissipating energy at a specific frequency, with a high Q indicating low energy loss and suitability for low-power, stable applications.</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/delivering-big-switching-power-in-a-small-package-with-sic-fets-0001</t>
+          <t>https://www.rfglobalnet.com/doc/high-q-capacitors-roles-and-specifications-0001</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Future-Ready Mobility: Small Cells, DAS, And Crafting A Future-Ready Mobility Landscape</t>
+          <t>Delivering Big Switching Power In A Small Package With SiC FETs</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>9/11/2023</t>
+          <t>9/12/2023</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Learn to equip buildings, campuses, and areas with a strong mobile network that supports emerging cellular technologies. Integrate small cells and DAS for a future-ready investment.</t>
+          <t>New SiC and GaN semiconductor switches offer better efficiency and smaller size than silicon-based parts. Qorvo's 750V SiC-FET in a compact TOLL package can greatly benefit your design.</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>DAS (ORG)</t>
+          <t>GaN (ORG), Qorvo (GPE)</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/future-ready-mobility-small-cells-das-and-crafting-a-future-ready-mobility-landscape-0001</t>
+          <t>https://www.rfglobalnet.com/doc/delivering-big-switching-power-in-a-small-package-with-sic-fets-0001</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>What Are Decoupling Capacitors?</t>
+          <t>Future-Ready Mobility: Small Cells, DAS, And Crafting A Future-Ready Mobility Landscape</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>9/1/2023</t>
+          <t>9/11/2023</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Decoupling capacitors play a crucial role in electronic circuits by effectively isolating AC and DC signals, providing clean and stable power to minimize malfunctions, noise coupling, and signal integrity issues.</t>
+          <t>Learn to equip buildings, campuses, and areas with a strong mobile network that supports emerging cellular technologies. Integrate small cells and DAS for a future-ready investment.</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>AC (ORG), DC (GPE)</t>
+          <t>DAS (ORG)</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/what-are-decoupling-capacitors-0001</t>
+          <t>https://www.rfglobalnet.com/doc/future-ready-mobility-small-cells-das-and-crafting-a-future-ready-mobility-landscape-0001</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Medical-Grade Capacitors For Implantable Device Design</t>
+          <t>What Are Decoupling Capacitors?</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2844,171 +2844,171 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>With 10% of Americans set to receive implantable devices, high-reliability components are crucial. Learn how our medical-grade capacitors streamline production while ensuring long-term integrity.</t>
+          <t>Decoupling capacitors play a crucial role in electronic circuits by effectively isolating AC and DC signals, providing clean and stable power to minimize malfunctions, noise coupling, and signal integrity issues.</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>10% (PERCENT), Americans (NORP)</t>
+          <t>AC (ORG), DC (GPE)</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/introducing-the-md-series-of-medical-grade-capacitors-for-implantable-device-design-0001</t>
+          <t>https://www.rfglobalnet.com/doc/what-are-decoupling-capacitors-0001</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Marki Microwave Expands Its Product Portfolio By Acquiring Precision Millimeter Wave</t>
+          <t>Medical-Grade Capacitors For Implantable Device Design</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>8/23/2023</t>
+          <t>9/1/2023</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Marki Microwave is pleased to announce it has expanded its product portfolio by acquiring the waveguide business of Precision Millimeter Wave.</t>
+          <t>With 10% of Americans set to receive implantable devices, high-reliability components are crucial. Learn how our medical-grade capacitors streamline production while ensuring long-term integrity.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Marki Microwave (PERSON), Millimeter Wave (PERSON)</t>
+          <t>10% (PERCENT), Americans (NORP)</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/marki-microwave-expands-its-product-portfolio-by-acquiring-waveguide-business-precision-millimeter-wave-0001</t>
+          <t>https://www.rfglobalnet.com/doc/introducing-the-md-series-of-medical-grade-capacitors-for-implantable-device-design-0001</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>mmWave Chip, Package, And Board Beamforming Solutions</t>
+          <t>Marki Microwave Expands Its Product Portfolio By Acquiring Precision Millimeter Wave</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>8/17/2023</t>
+          <t>8/23/2023</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>RF front-end architectures get increasingly intricate with each communication systems generation. This leads to greater densification and miniaturization via innovations in system-in-package (SiP) design.</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr"/>
+          <t>Marki Microwave is pleased to announce it has expanded its product portfolio by acquiring the waveguide business of Precision Millimeter Wave.</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Marki Microwave (PERSON), Millimeter Wave (PERSON)</t>
+        </is>
+      </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/mmwave-chip-package-and-board-beamforming-solutions-0001</t>
+          <t>https://www.rfglobalnet.com/doc/marki-microwave-expands-its-product-portfolio-by-acquiring-waveguide-business-precision-millimeter-wave-0001</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>A Fast Indoor Coverage Prediction Scheme At 60 GHz Based On Image Processing, Geometrical Optics, And Transport Theory</t>
+          <t>mmWave Chip, Package, And Board Beamforming Solutions</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>8/14/2023</t>
+          <t>8/17/2023</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>In this paper, we develop a fast and approximate prediction scheme for indoor path loss using digital image processing, geometrical optics, and transport theory.</t>
+          <t>RF front-end architectures get increasingly intricate with each communication systems generation. This leads to greater densification and miniaturization via innovations in system-in-package (SiP) design.</t>
         </is>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/a-fast-indoor-coverage-prediction-scheme-at-ghz-based-on-image-processing-geometrical-optics-and-transport-theory-0001</t>
+          <t>https://www.rfglobalnet.com/doc/mmwave-chip-package-and-board-beamforming-solutions-0001</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>The Many Jobs Of A Capacitor In RF And Microwave</t>
+          <t>A Fast Indoor Coverage Prediction Scheme At 60 GHz Based On Image Processing, Geometrical Optics, And Transport Theory</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>8/9/2023</t>
+          <t>8/14/2023</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>With many options for configurations and applications, capacitors support a variety of functions in RF and microwave circuits. Here are some examples of key roles they play in these applications.</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>RF (ORG)</t>
-        </is>
-      </c>
+          <t>In this paper, we develop a fast and approximate prediction scheme for indoor path loss using digital image processing, geometrical optics, and transport theory.</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/the-many-jobs-of-a-capacitor-in-rf-and-microwave-0001</t>
+          <t>https://www.rfglobalnet.com/doc/a-fast-indoor-coverage-prediction-scheme-at-ghz-based-on-image-processing-geometrical-optics-and-transport-theory-0001</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Automotive ADAS And Automated Driving</t>
+          <t>The Many Jobs Of A Capacitor In RF And Microwave</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>8/7/2023</t>
+          <t>8/9/2023</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>ADAS systems assist drivers with steering, braking, or acceleration functions to increase safety for all. They vary in complexity and are paving the way for fully autonomous vehicles.</t>
+          <t>With many options for configurations and applications, capacitors support a variety of functions in RF and microwave circuits. Here are some examples of key roles they play in these applications.</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>ADAS (ORG)</t>
+          <t>RF (ORG)</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/automotive-adas-and-automated-driving-0001</t>
+          <t>https://www.rfglobalnet.com/doc/the-many-jobs-of-a-capacitor-in-rf-and-microwave-0001</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>What Are EMI Filters?</t>
+          <t>Automotive ADAS And Automated Driving</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>8/2/2023</t>
+          <t>8/7/2023</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>An EMI filter is used to mitigate undesirable electromagnetic emissions or disturbances that can disrupt electronic systems, ensuring electromagnetic compatibility in the same environment.</t>
+          <t>ADAS systems assist drivers with steering, braking, or acceleration functions to increase safety for all. They vary in complexity and are paving the way for fully autonomous vehicles.</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>EMI (ORG)</t>
+          <t>ADAS (ORG)</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>https://www.rfglobalnet.com/doc/what-are-emi-filters-0001</t>
+          <t>https://www.rfglobalnet.com/doc/automotive-adas-and-automated-driving-0001</t>
         </is>
       </c>
     </row>

</xml_diff>